<commit_message>
Update excel template for vaccine inputs
</commit_message>
<xml_diff>
--- a/inst/extdata/template.xlsx
+++ b/inst/extdata/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/jsLEMMA/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brans\Desktop\LEMMA\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD6DC00-9ACE-4244-A286-B58BF337A39E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3C228A-D9D8-4715-8E91-502795A1B18D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="740" windowWidth="29440" windowHeight="17100" activeTab="1" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
+    <workbookView xWindow="18465" yWindow="3060" windowWidth="22095" windowHeight="21255" activeTab="5" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters with Distributions" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Model Inputs" sheetId="2" r:id="rId3"/>
     <sheet name="Data" sheetId="3" r:id="rId4"/>
     <sheet name="PUI Details" sheetId="7" r:id="rId5"/>
-    <sheet name="Internal" sheetId="4" r:id="rId6"/>
+    <sheet name="Vaccine" sheetId="8" r:id="rId6"/>
+    <sheet name="Internal" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
   <si>
     <t>Number of Days from Infection to Becoming Infectious (Latent Period)</t>
   </si>
@@ -303,13 +304,55 @@
   </si>
   <si>
     <t>skip2</t>
+  </si>
+  <si>
+    <t>First Date of Vaccination</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Shots Administered Per Day</t>
+  </si>
+  <si>
+    <t>Effectiveness of Vaccine Against Hospitalization</t>
+  </si>
+  <si>
+    <t>duration_natural</t>
+  </si>
+  <si>
+    <t>duration_vaccinated</t>
+  </si>
+  <si>
+    <t>shots.start</t>
+  </si>
+  <si>
+    <t>shots.per.day</t>
+  </si>
+  <si>
+    <t>Effectiveness of Vaccine Against Transmission</t>
+  </si>
+  <si>
+    <t>efficacy.against.hospitalization</t>
+  </si>
+  <si>
+    <t>efficacy.against.transmission</t>
+  </si>
+  <si>
+    <t>Duration of Vaccinated Immunity (Days)</t>
+  </si>
+  <si>
+    <t>Duration of Natural Immunity (Days)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -366,8 +409,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +452,11 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -473,11 +534,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -561,6 +623,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,8 +650,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -903,18 +971,18 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="28" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="62.5" style="2" customWidth="1"/>
-    <col min="3" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
@@ -928,7 +996,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>73</v>
       </c>
@@ -942,7 +1010,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>74</v>
       </c>
@@ -956,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>45</v>
       </c>
@@ -970,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>46</v>
       </c>
@@ -984,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>47</v>
       </c>
@@ -998,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>48</v>
       </c>
@@ -1012,7 +1080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>44</v>
       </c>
@@ -1026,7 +1094,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>51</v>
       </c>
@@ -1040,7 +1108,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>52</v>
       </c>
@@ -1073,33 +1141,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5372A5C3-523B-5F40-A7DB-9F78D72AADAB}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:8" s="26" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:8" s="26" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>35</v>
       </c>
@@ -1122,7 +1190,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>67</v>
       </c>
@@ -1148,7 +1216,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43897</v>
       </c>
@@ -1171,7 +1239,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43907</v>
       </c>
@@ -1219,16 +1287,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.625" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1239,7 +1307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1250,7 +1318,7 @@
         <v>883305</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1261,7 +1329,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1295,56 +1363,56 @@
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="3" customWidth="1"/>
-    <col min="4" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="3" customWidth="1"/>
+    <col min="4" max="7" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="3" customWidth="1"/>
     <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="45.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="15" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="36"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="39" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="39"/>
-    </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="40"/>
+    </row>
+    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="44" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="40" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="40"/>
-    </row>
-    <row r="3" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="41"/>
+    </row>
+    <row r="3" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1373,7 +1441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>28</v>
       </c>
@@ -1402,7 +1470,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>43913</v>
       </c>
@@ -1423,7 +1491,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>43914</v>
       </c>
@@ -1444,7 +1512,7 @@
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>43915</v>
       </c>
@@ -1465,7 +1533,7 @@
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>43916</v>
       </c>
@@ -1486,7 +1554,7 @@
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>43917</v>
       </c>
@@ -1507,7 +1575,7 @@
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>43918</v>
       </c>
@@ -1528,7 +1596,7 @@
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>43919</v>
       </c>
@@ -1549,7 +1617,7 @@
       <c r="H11" s="35"/>
       <c r="I11" s="34"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>43920</v>
       </c>
@@ -1566,7 +1634,7 @@
       <c r="H12" s="35"/>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>43921</v>
       </c>
@@ -1587,7 +1655,7 @@
       <c r="H13" s="35"/>
       <c r="I13" s="34"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>43922</v>
       </c>
@@ -1610,7 +1678,7 @@
       <c r="H14" s="35"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>43923</v>
       </c>
@@ -1633,7 +1701,7 @@
       <c r="H15" s="35"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>43924</v>
       </c>
@@ -1656,7 +1724,7 @@
       <c r="H16" s="35"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>43925</v>
       </c>
@@ -1679,7 +1747,7 @@
       <c r="H17" s="35"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>43926</v>
       </c>
@@ -1702,7 +1770,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>43927</v>
       </c>
@@ -1725,7 +1793,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="34"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>43928</v>
       </c>
@@ -1748,7 +1816,7 @@
       <c r="H20" s="35"/>
       <c r="I20" s="34"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>43929</v>
       </c>
@@ -1771,7 +1839,7 @@
       <c r="H21" s="35"/>
       <c r="I21" s="34"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>43930</v>
       </c>
@@ -1794,7 +1862,7 @@
       <c r="H22" s="35"/>
       <c r="I22" s="34"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>43931</v>
       </c>
@@ -1817,7 +1885,7 @@
       <c r="H23" s="35"/>
       <c r="I23" s="34"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>43932</v>
       </c>
@@ -1840,7 +1908,7 @@
       <c r="H24" s="35"/>
       <c r="I24" s="34"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>43933</v>
       </c>
@@ -1863,7 +1931,7 @@
       <c r="H25" s="35"/>
       <c r="I25" s="34"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>43934</v>
       </c>
@@ -1886,7 +1954,7 @@
       <c r="H26" s="35"/>
       <c r="I26" s="34"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>43935</v>
       </c>
@@ -1909,7 +1977,7 @@
       <c r="H27" s="35"/>
       <c r="I27" s="34"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>43936</v>
       </c>
@@ -1932,7 +2000,7 @@
       <c r="H28" s="35"/>
       <c r="I28" s="34"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>43937</v>
       </c>
@@ -1955,7 +2023,7 @@
       <c r="H29" s="35"/>
       <c r="I29" s="34"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>43938</v>
       </c>
@@ -1978,7 +2046,7 @@
       <c r="H30" s="35"/>
       <c r="I30" s="34"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <v>43939</v>
       </c>
@@ -2001,7 +2069,7 @@
       <c r="H31" s="35"/>
       <c r="I31" s="34"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <v>43940</v>
       </c>
@@ -2024,7 +2092,7 @@
       <c r="H32" s="35"/>
       <c r="I32" s="34"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>43941</v>
       </c>
@@ -2047,7 +2115,7 @@
       <c r="H33" s="35"/>
       <c r="I33" s="34"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>43942</v>
       </c>
@@ -2070,7 +2138,7 @@
       <c r="H34" s="35"/>
       <c r="I34" s="34"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>43943</v>
       </c>
@@ -2093,7 +2161,7 @@
       <c r="H35" s="35"/>
       <c r="I35" s="34"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>43944</v>
       </c>
@@ -2116,7 +2184,7 @@
       <c r="H36" s="35"/>
       <c r="I36" s="34"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
         <v>43945</v>
       </c>
@@ -2139,7 +2207,7 @@
       <c r="H37" s="35"/>
       <c r="I37" s="34"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>43946</v>
       </c>
@@ -2162,7 +2230,7 @@
       <c r="H38" s="35"/>
       <c r="I38" s="34"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="18">
         <v>43947</v>
       </c>
@@ -2185,7 +2253,7 @@
       <c r="H39" s="35"/>
       <c r="I39" s="34"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>43948</v>
       </c>
@@ -2208,7 +2276,7 @@
       <c r="H40" s="35"/>
       <c r="I40" s="34"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>43949</v>
       </c>
@@ -2231,7 +2299,7 @@
       <c r="H41" s="35"/>
       <c r="I41" s="34"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <v>43950</v>
       </c>
@@ -2254,7 +2322,7 @@
       <c r="H42" s="35"/>
       <c r="I42" s="34"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>43951</v>
       </c>
@@ -2277,7 +2345,7 @@
       <c r="H43" s="35"/>
       <c r="I43" s="34"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <v>43952</v>
       </c>
@@ -2300,7 +2368,7 @@
       <c r="H44" s="35"/>
       <c r="I44" s="34"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>43953</v>
       </c>
@@ -2323,7 +2391,7 @@
       <c r="H45" s="35"/>
       <c r="I45" s="34"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>43954</v>
       </c>
@@ -2346,7 +2414,7 @@
       <c r="H46" s="35"/>
       <c r="I46" s="34"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>43955</v>
       </c>
@@ -2369,7 +2437,7 @@
       <c r="H47" s="35"/>
       <c r="I47" s="34"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>43956</v>
       </c>
@@ -2392,7 +2460,7 @@
       <c r="H48" s="35"/>
       <c r="I48" s="34"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>43957</v>
       </c>
@@ -2415,7 +2483,7 @@
       <c r="H49" s="35"/>
       <c r="I49" s="34"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>43958</v>
       </c>
@@ -2438,7 +2506,7 @@
       <c r="H50" s="35"/>
       <c r="I50" s="34"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>43959</v>
       </c>
@@ -2461,7 +2529,7 @@
       <c r="H51" s="35"/>
       <c r="I51" s="34"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
         <v>43960</v>
       </c>
@@ -2484,7 +2552,7 @@
       <c r="H52" s="35"/>
       <c r="I52" s="34"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
         <v>43961</v>
       </c>
@@ -2507,7 +2575,7 @@
       <c r="H53" s="35"/>
       <c r="I53" s="34"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
         <v>43962</v>
       </c>
@@ -2530,7 +2598,7 @@
       <c r="H54" s="35"/>
       <c r="I54" s="34"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="18">
         <v>43963</v>
       </c>
@@ -2553,7 +2621,7 @@
       <c r="H55" s="35"/>
       <c r="I55" s="34"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
         <v>43964</v>
       </c>
@@ -2576,7 +2644,7 @@
       <c r="H56" s="35"/>
       <c r="I56" s="34"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
         <v>43965</v>
       </c>
@@ -2599,7 +2667,7 @@
       <c r="H57" s="35"/>
       <c r="I57" s="34"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <v>43966</v>
       </c>
@@ -2622,7 +2690,7 @@
       <c r="H58" s="35"/>
       <c r="I58" s="34"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <v>43967</v>
       </c>
@@ -2645,7 +2713,7 @@
       <c r="H59" s="35"/>
       <c r="I59" s="34"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <v>43968</v>
       </c>
@@ -2668,7 +2736,7 @@
       <c r="H60" s="35"/>
       <c r="I60" s="34"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <v>43969</v>
       </c>
@@ -2691,7 +2759,7 @@
       <c r="H61" s="35"/>
       <c r="I61" s="34"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <v>43970</v>
       </c>
@@ -2714,7 +2782,7 @@
       <c r="H62" s="35"/>
       <c r="I62" s="34"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
         <v>43971</v>
       </c>
@@ -2737,7 +2805,7 @@
       <c r="H63" s="35"/>
       <c r="I63" s="34"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
         <v>43972</v>
       </c>
@@ -2760,7 +2828,7 @@
       <c r="H64" s="35"/>
       <c r="I64" s="34"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="22">
         <v>43973</v>
       </c>
@@ -2783,7 +2851,7 @@
       <c r="H65" s="35"/>
       <c r="I65" s="34"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="22">
         <v>43974</v>
       </c>
@@ -2806,7 +2874,7 @@
       <c r="H66" s="34"/>
       <c r="I66" s="34"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="22">
         <v>43975</v>
       </c>
@@ -2829,7 +2897,7 @@
       <c r="H67" s="34"/>
       <c r="I67" s="34"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="22">
         <v>43976</v>
       </c>
@@ -2852,7 +2920,7 @@
       <c r="H68" s="34"/>
       <c r="I68" s="34"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="22">
         <v>43977</v>
       </c>
@@ -2875,7 +2943,7 @@
       <c r="H69" s="34"/>
       <c r="I69" s="34"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="22">
         <v>43978</v>
       </c>
@@ -2898,7 +2966,7 @@
       <c r="H70" s="34"/>
       <c r="I70" s="34"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
         <v>43979</v>
       </c>
@@ -2921,7 +2989,7 @@
       <c r="H71" s="34"/>
       <c r="I71" s="34"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
         <v>43980</v>
       </c>
@@ -2944,7 +3012,7 @@
       <c r="H72" s="34"/>
       <c r="I72" s="34"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="18">
         <v>43981</v>
       </c>
@@ -2967,7 +3035,7 @@
       <c r="H73" s="34"/>
       <c r="I73" s="34"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="18">
         <v>43982</v>
       </c>
@@ -2990,7 +3058,7 @@
       <c r="H74" s="34"/>
       <c r="I74" s="34"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="18">
         <v>43983</v>
       </c>
@@ -3013,7 +3081,7 @@
       <c r="H75" s="34"/>
       <c r="I75" s="34"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="18">
         <v>43984</v>
       </c>
@@ -3036,7 +3104,7 @@
       <c r="H76" s="34"/>
       <c r="I76" s="34"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="18">
         <v>43985</v>
       </c>
@@ -3059,7 +3127,7 @@
       <c r="H77" s="34"/>
       <c r="I77" s="34"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
         <v>43986</v>
       </c>
@@ -3082,7 +3150,7 @@
       <c r="H78" s="34"/>
       <c r="I78" s="34"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
         <v>43987</v>
       </c>
@@ -3105,7 +3173,7 @@
       <c r="H79" s="34"/>
       <c r="I79" s="34"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
         <v>43988</v>
       </c>
@@ -3128,7 +3196,7 @@
       <c r="H80" s="34"/>
       <c r="I80" s="34"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="18">
         <v>43989</v>
       </c>
@@ -3151,7 +3219,7 @@
       <c r="H81" s="34"/>
       <c r="I81" s="34"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
         <v>43990</v>
       </c>
@@ -3174,7 +3242,7 @@
       <c r="H82" s="34"/>
       <c r="I82" s="34"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="18"/>
       <c r="B83" s="34"/>
       <c r="C83" s="34"/>
@@ -3185,7 +3253,7 @@
       <c r="H83" s="34"/>
       <c r="I83" s="34"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="18"/>
       <c r="B84" s="34"/>
       <c r="C84" s="34"/>
@@ -3196,7 +3264,7 @@
       <c r="H84" s="34"/>
       <c r="I84" s="34"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="18"/>
       <c r="B85" s="34"/>
       <c r="C85" s="34"/>
@@ -3207,7 +3275,7 @@
       <c r="H85" s="34"/>
       <c r="I85" s="34"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="18"/>
       <c r="B86" s="34"/>
       <c r="C86" s="34"/>
@@ -3218,7 +3286,7 @@
       <c r="H86" s="34"/>
       <c r="I86" s="34"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="18"/>
       <c r="B87" s="34"/>
       <c r="C87" s="34"/>
@@ -3229,7 +3297,7 @@
       <c r="H87" s="34"/>
       <c r="I87" s="34"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="18"/>
       <c r="B88" s="34"/>
       <c r="C88" s="34"/>
@@ -3240,7 +3308,7 @@
       <c r="H88" s="34"/>
       <c r="I88" s="34"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="18"/>
       <c r="B89" s="34"/>
       <c r="C89" s="34"/>
@@ -3251,7 +3319,7 @@
       <c r="H89" s="34"/>
       <c r="I89" s="34"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="18"/>
       <c r="B90" s="34"/>
       <c r="C90" s="34"/>
@@ -3262,7 +3330,7 @@
       <c r="H90" s="34"/>
       <c r="I90" s="34"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="18"/>
       <c r="B91" s="34"/>
       <c r="C91" s="34"/>
@@ -3273,7 +3341,7 @@
       <c r="H91" s="34"/>
       <c r="I91" s="34"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="18"/>
       <c r="B92" s="34"/>
       <c r="C92" s="34"/>
@@ -3284,7 +3352,7 @@
       <c r="H92" s="34"/>
       <c r="I92" s="34"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="18"/>
       <c r="B93" s="34"/>
       <c r="C93" s="34"/>
@@ -3295,7 +3363,7 @@
       <c r="H93" s="34"/>
       <c r="I93" s="34"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="18"/>
       <c r="B94" s="34"/>
       <c r="C94" s="34"/>
@@ -3306,7 +3374,7 @@
       <c r="H94" s="34"/>
       <c r="I94" s="34"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="18"/>
       <c r="B95" s="34"/>
       <c r="C95" s="34"/>
@@ -3317,7 +3385,7 @@
       <c r="H95" s="34"/>
       <c r="I95" s="34"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="18"/>
       <c r="B96" s="34"/>
       <c r="C96" s="34"/>
@@ -3328,7 +3396,7 @@
       <c r="H96" s="34"/>
       <c r="I96" s="34"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="18"/>
       <c r="B97" s="34"/>
       <c r="C97" s="34"/>
@@ -3339,7 +3407,7 @@
       <c r="H97" s="34"/>
       <c r="I97" s="34"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="18"/>
       <c r="B98" s="34"/>
       <c r="C98" s="34"/>
@@ -3350,7 +3418,7 @@
       <c r="H98" s="34"/>
       <c r="I98" s="34"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="18"/>
       <c r="B99" s="34"/>
       <c r="C99" s="34"/>
@@ -3361,7 +3429,7 @@
       <c r="H99" s="34"/>
       <c r="I99" s="34"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="18"/>
       <c r="B100" s="34"/>
       <c r="C100" s="34"/>
@@ -3372,7 +3440,7 @@
       <c r="H100" s="34"/>
       <c r="I100" s="34"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="18"/>
       <c r="B101" s="34"/>
       <c r="C101" s="34"/>
@@ -3383,7 +3451,7 @@
       <c r="H101" s="34"/>
       <c r="I101" s="34"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="18"/>
       <c r="B102" s="34"/>
       <c r="C102" s="34"/>
@@ -3394,7 +3462,7 @@
       <c r="H102" s="34"/>
       <c r="I102" s="34"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="18"/>
       <c r="B103" s="34"/>
       <c r="C103" s="34"/>
@@ -3405,7 +3473,7 @@
       <c r="H103" s="34"/>
       <c r="I103" s="34"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="18"/>
       <c r="B104" s="34"/>
       <c r="C104" s="34"/>
@@ -3416,7 +3484,7 @@
       <c r="H104" s="34"/>
       <c r="I104" s="34"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="18"/>
       <c r="B105" s="34"/>
       <c r="C105" s="34"/>
@@ -3427,7 +3495,7 @@
       <c r="H105" s="34"/>
       <c r="I105" s="34"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="18"/>
       <c r="B106" s="34"/>
       <c r="C106" s="34"/>
@@ -3438,7 +3506,7 @@
       <c r="H106" s="34"/>
       <c r="I106" s="34"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="18"/>
       <c r="B107" s="34"/>
       <c r="C107" s="34"/>
@@ -3449,7 +3517,7 @@
       <c r="H107" s="34"/>
       <c r="I107" s="34"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="18"/>
       <c r="B108" s="34"/>
       <c r="C108" s="34"/>
@@ -3460,7 +3528,7 @@
       <c r="H108" s="34"/>
       <c r="I108" s="34"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="18"/>
       <c r="B109" s="34"/>
       <c r="C109" s="34"/>
@@ -3471,7 +3539,7 @@
       <c r="H109" s="34"/>
       <c r="I109" s="34"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="18"/>
       <c r="B110" s="34"/>
       <c r="C110" s="34"/>
@@ -3482,7 +3550,7 @@
       <c r="H110" s="34"/>
       <c r="I110" s="34"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="18"/>
       <c r="B111" s="34"/>
       <c r="C111" s="34"/>
@@ -3493,7 +3561,7 @@
       <c r="H111" s="34"/>
       <c r="I111" s="34"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="18"/>
       <c r="B112" s="34"/>
       <c r="C112" s="34"/>
@@ -3504,7 +3572,7 @@
       <c r="H112" s="34"/>
       <c r="I112" s="34"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="18"/>
       <c r="B113" s="34"/>
       <c r="C113" s="34"/>
@@ -3515,7 +3583,7 @@
       <c r="H113" s="34"/>
       <c r="I113" s="34"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="18"/>
       <c r="B114" s="34"/>
       <c r="C114" s="34"/>
@@ -3526,7 +3594,7 @@
       <c r="H114" s="34"/>
       <c r="I114" s="34"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="18"/>
       <c r="B115" s="34"/>
       <c r="C115" s="34"/>
@@ -3537,7 +3605,7 @@
       <c r="H115" s="34"/>
       <c r="I115" s="34"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="18"/>
       <c r="B116" s="34"/>
       <c r="C116" s="34"/>
@@ -3548,7 +3616,7 @@
       <c r="H116" s="34"/>
       <c r="I116" s="34"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="18"/>
       <c r="B117" s="34"/>
       <c r="C117" s="34"/>
@@ -3559,7 +3627,7 @@
       <c r="H117" s="34"/>
       <c r="I117" s="34"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="18"/>
       <c r="B118" s="34"/>
       <c r="C118" s="34"/>
@@ -3570,7 +3638,7 @@
       <c r="H118" s="34"/>
       <c r="I118" s="34"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="18"/>
       <c r="B119" s="34"/>
       <c r="C119" s="34"/>
@@ -3581,7 +3649,7 @@
       <c r="H119" s="34"/>
       <c r="I119" s="34"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="18"/>
       <c r="B120" s="34"/>
       <c r="C120" s="34"/>
@@ -3592,7 +3660,7 @@
       <c r="H120" s="34"/>
       <c r="I120" s="34"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="18"/>
       <c r="B121" s="34"/>
       <c r="C121" s="34"/>
@@ -3603,7 +3671,7 @@
       <c r="H121" s="34"/>
       <c r="I121" s="34"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="18"/>
       <c r="B122" s="34"/>
       <c r="C122" s="34"/>
@@ -3614,7 +3682,7 @@
       <c r="H122" s="34"/>
       <c r="I122" s="34"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="18"/>
       <c r="B123" s="34"/>
       <c r="C123" s="34"/>
@@ -3625,7 +3693,7 @@
       <c r="H123" s="34"/>
       <c r="I123" s="34"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="18"/>
       <c r="B124" s="34"/>
       <c r="C124" s="34"/>
@@ -3636,7 +3704,7 @@
       <c r="H124" s="34"/>
       <c r="I124" s="34"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="18"/>
       <c r="B125" s="34"/>
       <c r="C125" s="34"/>
@@ -3647,7 +3715,7 @@
       <c r="H125" s="34"/>
       <c r="I125" s="34"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="18"/>
       <c r="B126" s="34"/>
       <c r="C126" s="34"/>
@@ -3658,7 +3726,7 @@
       <c r="H126" s="34"/>
       <c r="I126" s="34"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="18"/>
       <c r="B127" s="34"/>
       <c r="C127" s="34"/>
@@ -3669,7 +3737,7 @@
       <c r="H127" s="34"/>
       <c r="I127" s="34"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="18"/>
       <c r="B128" s="34"/>
       <c r="C128" s="34"/>
@@ -3680,7 +3748,7 @@
       <c r="H128" s="34"/>
       <c r="I128" s="34"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="18"/>
       <c r="B129" s="34"/>
       <c r="C129" s="34"/>
@@ -3691,7 +3759,7 @@
       <c r="H129" s="34"/>
       <c r="I129" s="34"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="18"/>
       <c r="B130" s="34"/>
       <c r="C130" s="34"/>
@@ -3702,7 +3770,7 @@
       <c r="H130" s="34"/>
       <c r="I130" s="34"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="18"/>
       <c r="B131" s="34"/>
       <c r="C131" s="34"/>
@@ -3713,7 +3781,7 @@
       <c r="H131" s="34"/>
       <c r="I131" s="34"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="18"/>
       <c r="B132" s="34"/>
       <c r="C132" s="34"/>
@@ -3724,7 +3792,7 @@
       <c r="H132" s="34"/>
       <c r="I132" s="34"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="18"/>
       <c r="B133" s="34"/>
       <c r="C133" s="34"/>
@@ -3735,7 +3803,7 @@
       <c r="H133" s="34"/>
       <c r="I133" s="34"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="18"/>
       <c r="B134" s="34"/>
       <c r="C134" s="34"/>
@@ -3746,7 +3814,7 @@
       <c r="H134" s="34"/>
       <c r="I134" s="34"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="18"/>
       <c r="B135" s="34"/>
       <c r="C135" s="34"/>
@@ -3757,7 +3825,7 @@
       <c r="H135" s="34"/>
       <c r="I135" s="34"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="18"/>
       <c r="B136" s="34"/>
       <c r="C136" s="34"/>
@@ -3768,7 +3836,7 @@
       <c r="H136" s="34"/>
       <c r="I136" s="34"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="18"/>
       <c r="B137" s="34"/>
       <c r="C137" s="34"/>
@@ -3779,7 +3847,7 @@
       <c r="H137" s="34"/>
       <c r="I137" s="34"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="18"/>
       <c r="B138" s="34"/>
       <c r="C138" s="34"/>
@@ -3790,7 +3858,7 @@
       <c r="H138" s="34"/>
       <c r="I138" s="34"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="18"/>
       <c r="B139" s="34"/>
       <c r="C139" s="34"/>
@@ -3801,7 +3869,7 @@
       <c r="H139" s="34"/>
       <c r="I139" s="34"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="18"/>
       <c r="B140" s="34"/>
       <c r="C140" s="34"/>
@@ -3812,7 +3880,7 @@
       <c r="H140" s="34"/>
       <c r="I140" s="34"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="18"/>
       <c r="B141" s="34"/>
       <c r="C141" s="34"/>
@@ -3823,7 +3891,7 @@
       <c r="H141" s="34"/>
       <c r="I141" s="34"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="18"/>
       <c r="B142" s="34"/>
       <c r="C142" s="34"/>
@@ -3834,7 +3902,7 @@
       <c r="H142" s="34"/>
       <c r="I142" s="34"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="18"/>
       <c r="B143" s="34"/>
       <c r="C143" s="34"/>
@@ -3845,7 +3913,7 @@
       <c r="H143" s="34"/>
       <c r="I143" s="34"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="18"/>
       <c r="B144" s="34"/>
       <c r="C144" s="34"/>
@@ -3856,7 +3924,7 @@
       <c r="H144" s="34"/>
       <c r="I144" s="34"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="18"/>
       <c r="B145" s="34"/>
       <c r="C145" s="34"/>
@@ -3867,7 +3935,7 @@
       <c r="H145" s="34"/>
       <c r="I145" s="34"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="18"/>
       <c r="B146" s="34"/>
       <c r="C146" s="34"/>
@@ -3878,7 +3946,7 @@
       <c r="H146" s="34"/>
       <c r="I146" s="34"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="18"/>
       <c r="B147" s="34"/>
       <c r="C147" s="34"/>
@@ -3889,7 +3957,7 @@
       <c r="H147" s="34"/>
       <c r="I147" s="34"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="18"/>
       <c r="B148" s="34"/>
       <c r="C148" s="34"/>
@@ -3900,7 +3968,7 @@
       <c r="H148" s="34"/>
       <c r="I148" s="34"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="18"/>
       <c r="B149" s="34"/>
       <c r="C149" s="34"/>
@@ -3911,7 +3979,7 @@
       <c r="H149" s="34"/>
       <c r="I149" s="34"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="18"/>
       <c r="B150" s="34"/>
       <c r="C150" s="34"/>
@@ -3922,7 +3990,7 @@
       <c r="H150" s="34"/>
       <c r="I150" s="34"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="18"/>
       <c r="B151" s="34"/>
       <c r="C151" s="34"/>
@@ -3933,7 +4001,7 @@
       <c r="H151" s="34"/>
       <c r="I151" s="34"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="18"/>
       <c r="B152" s="34"/>
       <c r="C152" s="34"/>
@@ -3944,7 +4012,7 @@
       <c r="H152" s="34"/>
       <c r="I152" s="34"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="18"/>
       <c r="B153" s="34"/>
       <c r="C153" s="34"/>
@@ -3955,7 +4023,7 @@
       <c r="H153" s="34"/>
       <c r="I153" s="34"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="18"/>
       <c r="B154" s="34"/>
       <c r="C154" s="34"/>
@@ -3966,7 +4034,7 @@
       <c r="H154" s="34"/>
       <c r="I154" s="34"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="18"/>
       <c r="B155" s="34"/>
       <c r="C155" s="34"/>
@@ -3977,7 +4045,7 @@
       <c r="H155" s="34"/>
       <c r="I155" s="34"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="18"/>
       <c r="B156" s="34"/>
       <c r="C156" s="34"/>
@@ -3988,7 +4056,7 @@
       <c r="H156" s="34"/>
       <c r="I156" s="34"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="18"/>
       <c r="B157" s="34"/>
       <c r="C157" s="34"/>
@@ -3999,7 +4067,7 @@
       <c r="H157" s="34"/>
       <c r="I157" s="34"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="18"/>
       <c r="B158" s="34"/>
       <c r="C158" s="34"/>
@@ -4010,7 +4078,7 @@
       <c r="H158" s="34"/>
       <c r="I158" s="34"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="18"/>
       <c r="B159" s="34"/>
       <c r="C159" s="34"/>
@@ -4021,7 +4089,7 @@
       <c r="H159" s="34"/>
       <c r="I159" s="34"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="18"/>
       <c r="B160" s="34"/>
       <c r="C160" s="34"/>
@@ -4032,7 +4100,7 @@
       <c r="H160" s="34"/>
       <c r="I160" s="34"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="18"/>
       <c r="B161" s="34"/>
       <c r="C161" s="34"/>
@@ -4043,7 +4111,7 @@
       <c r="H161" s="34"/>
       <c r="I161" s="34"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="18"/>
       <c r="B162" s="34"/>
       <c r="C162" s="34"/>
@@ -4054,7 +4122,7 @@
       <c r="H162" s="34"/>
       <c r="I162" s="34"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="18"/>
       <c r="B163" s="34"/>
       <c r="C163" s="34"/>
@@ -4065,7 +4133,7 @@
       <c r="H163" s="34"/>
       <c r="I163" s="34"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="18"/>
       <c r="B164" s="34"/>
       <c r="C164" s="34"/>
@@ -4076,7 +4144,7 @@
       <c r="H164" s="34"/>
       <c r="I164" s="34"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="18"/>
       <c r="B165" s="34"/>
       <c r="C165" s="34"/>
@@ -4087,7 +4155,7 @@
       <c r="H165" s="34"/>
       <c r="I165" s="34"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="18"/>
       <c r="B166" s="34"/>
       <c r="C166" s="34"/>
@@ -4098,7 +4166,7 @@
       <c r="H166" s="34"/>
       <c r="I166" s="34"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="18"/>
       <c r="B167" s="34"/>
       <c r="C167" s="34"/>
@@ -4109,7 +4177,7 @@
       <c r="H167" s="34"/>
       <c r="I167" s="34"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="18"/>
       <c r="B168" s="34"/>
       <c r="C168" s="34"/>
@@ -4120,7 +4188,7 @@
       <c r="H168" s="34"/>
       <c r="I168" s="34"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="18"/>
       <c r="B169" s="34"/>
       <c r="C169" s="34"/>
@@ -4131,7 +4199,7 @@
       <c r="H169" s="34"/>
       <c r="I169" s="34"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="18"/>
       <c r="B170" s="34"/>
       <c r="C170" s="34"/>
@@ -4142,7 +4210,7 @@
       <c r="H170" s="34"/>
       <c r="I170" s="34"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="18"/>
       <c r="B171" s="34"/>
       <c r="C171" s="34"/>
@@ -4153,7 +4221,7 @@
       <c r="H171" s="34"/>
       <c r="I171" s="34"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="18"/>
       <c r="B172" s="34"/>
       <c r="C172" s="34"/>
@@ -4164,7 +4232,7 @@
       <c r="H172" s="34"/>
       <c r="I172" s="34"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="18"/>
       <c r="B173" s="34"/>
       <c r="C173" s="34"/>
@@ -4175,7 +4243,7 @@
       <c r="H173" s="34"/>
       <c r="I173" s="34"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="18"/>
       <c r="B174" s="34"/>
       <c r="C174" s="34"/>
@@ -4186,7 +4254,7 @@
       <c r="H174" s="34"/>
       <c r="I174" s="34"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="18"/>
       <c r="B175" s="34"/>
       <c r="C175" s="34"/>
@@ -4197,7 +4265,7 @@
       <c r="H175" s="34"/>
       <c r="I175" s="34"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="18"/>
       <c r="B176" s="34"/>
       <c r="C176" s="34"/>
@@ -4208,7 +4276,7 @@
       <c r="H176" s="34"/>
       <c r="I176" s="34"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="18"/>
       <c r="B177" s="34"/>
       <c r="C177" s="34"/>
@@ -4219,7 +4287,7 @@
       <c r="H177" s="34"/>
       <c r="I177" s="34"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="18"/>
       <c r="B178" s="34"/>
       <c r="C178" s="34"/>
@@ -4230,7 +4298,7 @@
       <c r="H178" s="34"/>
       <c r="I178" s="34"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="18"/>
       <c r="B179" s="34"/>
       <c r="C179" s="34"/>
@@ -4241,7 +4309,7 @@
       <c r="H179" s="34"/>
       <c r="I179" s="34"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="18"/>
       <c r="B180" s="34"/>
       <c r="C180" s="34"/>
@@ -4252,7 +4320,7 @@
       <c r="H180" s="34"/>
       <c r="I180" s="34"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="18"/>
       <c r="B181" s="34"/>
       <c r="C181" s="34"/>
@@ -4263,7 +4331,7 @@
       <c r="H181" s="34"/>
       <c r="I181" s="34"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="18"/>
       <c r="B182" s="34"/>
       <c r="C182" s="34"/>
@@ -4274,7 +4342,7 @@
       <c r="H182" s="34"/>
       <c r="I182" s="34"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="18"/>
       <c r="B183" s="34"/>
       <c r="C183" s="34"/>
@@ -4285,7 +4353,7 @@
       <c r="H183" s="34"/>
       <c r="I183" s="34"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="18"/>
       <c r="B184" s="34"/>
       <c r="C184" s="34"/>
@@ -4296,7 +4364,7 @@
       <c r="H184" s="34"/>
       <c r="I184" s="34"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="18"/>
       <c r="B185" s="34"/>
       <c r="C185" s="34"/>
@@ -4307,7 +4375,7 @@
       <c r="H185" s="34"/>
       <c r="I185" s="34"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="18"/>
       <c r="B186" s="34"/>
       <c r="C186" s="34"/>
@@ -4318,7 +4386,7 @@
       <c r="H186" s="34"/>
       <c r="I186" s="34"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="18"/>
       <c r="B187" s="34"/>
       <c r="C187" s="34"/>
@@ -4329,7 +4397,7 @@
       <c r="H187" s="34"/>
       <c r="I187" s="34"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="18"/>
       <c r="B188" s="34"/>
       <c r="C188" s="34"/>
@@ -4340,7 +4408,7 @@
       <c r="H188" s="34"/>
       <c r="I188" s="34"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="18"/>
       <c r="B189" s="34"/>
       <c r="C189" s="34"/>
@@ -4351,7 +4419,7 @@
       <c r="H189" s="34"/>
       <c r="I189" s="34"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="18"/>
       <c r="B190" s="34"/>
       <c r="C190" s="34"/>
@@ -4362,7 +4430,7 @@
       <c r="H190" s="34"/>
       <c r="I190" s="34"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="18"/>
       <c r="B191" s="34"/>
       <c r="C191" s="34"/>
@@ -4373,7 +4441,7 @@
       <c r="H191" s="34"/>
       <c r="I191" s="34"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="18"/>
       <c r="B192" s="34"/>
       <c r="C192" s="34"/>
@@ -4384,7 +4452,7 @@
       <c r="H192" s="34"/>
       <c r="I192" s="34"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="18"/>
       <c r="B193" s="34"/>
       <c r="C193" s="34"/>
@@ -4395,7 +4463,7 @@
       <c r="H193" s="34"/>
       <c r="I193" s="34"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="18"/>
       <c r="B194" s="34"/>
       <c r="C194" s="34"/>
@@ -4406,7 +4474,7 @@
       <c r="H194" s="34"/>
       <c r="I194" s="34"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="18"/>
       <c r="B195" s="34"/>
       <c r="C195" s="34"/>
@@ -4417,7 +4485,7 @@
       <c r="H195" s="34"/>
       <c r="I195" s="34"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="18"/>
       <c r="B196" s="34"/>
       <c r="C196" s="34"/>
@@ -4428,7 +4496,7 @@
       <c r="H196" s="34"/>
       <c r="I196" s="34"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="18"/>
       <c r="B197" s="34"/>
       <c r="C197" s="34"/>
@@ -4439,7 +4507,7 @@
       <c r="H197" s="34"/>
       <c r="I197" s="34"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="18"/>
       <c r="B198" s="34"/>
       <c r="C198" s="34"/>
@@ -4450,7 +4518,7 @@
       <c r="H198" s="34"/>
       <c r="I198" s="34"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="18"/>
       <c r="B199" s="34"/>
       <c r="C199" s="34"/>
@@ -4461,7 +4529,7 @@
       <c r="H199" s="34"/>
       <c r="I199" s="34"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="18"/>
       <c r="B200" s="34"/>
       <c r="C200" s="34"/>
@@ -4472,7 +4540,7 @@
       <c r="H200" s="34"/>
       <c r="I200" s="34"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="18"/>
       <c r="B201" s="34"/>
       <c r="C201" s="34"/>
@@ -4483,7 +4551,7 @@
       <c r="H201" s="34"/>
       <c r="I201" s="34"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="18"/>
       <c r="B202" s="34"/>
       <c r="C202" s="34"/>
@@ -4494,7 +4562,7 @@
       <c r="H202" s="34"/>
       <c r="I202" s="34"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="18"/>
       <c r="B203" s="34"/>
       <c r="C203" s="34"/>
@@ -4505,7 +4573,7 @@
       <c r="H203" s="34"/>
       <c r="I203" s="34"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="18"/>
       <c r="B204" s="34"/>
       <c r="C204" s="34"/>
@@ -4516,7 +4584,7 @@
       <c r="H204" s="34"/>
       <c r="I204" s="34"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="18"/>
       <c r="B205" s="34"/>
       <c r="C205" s="34"/>
@@ -4527,7 +4595,7 @@
       <c r="H205" s="34"/>
       <c r="I205" s="34"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="18"/>
       <c r="B206" s="34"/>
       <c r="C206" s="34"/>
@@ -4538,7 +4606,7 @@
       <c r="H206" s="34"/>
       <c r="I206" s="34"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="18"/>
       <c r="B207" s="34"/>
       <c r="C207" s="34"/>
@@ -4549,7 +4617,7 @@
       <c r="H207" s="34"/>
       <c r="I207" s="34"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="18"/>
       <c r="B208" s="34"/>
       <c r="C208" s="34"/>
@@ -4560,7 +4628,7 @@
       <c r="H208" s="34"/>
       <c r="I208" s="34"/>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="18"/>
       <c r="B209" s="34"/>
       <c r="C209" s="34"/>
@@ -4571,7 +4639,7 @@
       <c r="H209" s="34"/>
       <c r="I209" s="34"/>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="18"/>
       <c r="B210" s="34"/>
       <c r="C210" s="34"/>
@@ -4582,7 +4650,7 @@
       <c r="H210" s="34"/>
       <c r="I210" s="34"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="18"/>
       <c r="B211" s="34"/>
       <c r="C211" s="34"/>
@@ -4593,7 +4661,7 @@
       <c r="H211" s="34"/>
       <c r="I211" s="34"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="18"/>
       <c r="B212" s="34"/>
       <c r="C212" s="34"/>
@@ -4604,7 +4672,7 @@
       <c r="H212" s="34"/>
       <c r="I212" s="34"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="18"/>
       <c r="B213" s="34"/>
       <c r="C213" s="34"/>
@@ -4615,7 +4683,7 @@
       <c r="H213" s="34"/>
       <c r="I213" s="34"/>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="18"/>
       <c r="B214" s="34"/>
       <c r="C214" s="34"/>
@@ -4626,7 +4694,7 @@
       <c r="H214" s="34"/>
       <c r="I214" s="34"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="18"/>
       <c r="B215" s="34"/>
       <c r="C215" s="34"/>
@@ -4637,7 +4705,7 @@
       <c r="H215" s="34"/>
       <c r="I215" s="34"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="18"/>
       <c r="B216" s="34"/>
       <c r="C216" s="34"/>
@@ -4648,7 +4716,7 @@
       <c r="H216" s="34"/>
       <c r="I216" s="34"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="18"/>
       <c r="B217" s="34"/>
       <c r="C217" s="34"/>
@@ -4659,7 +4727,7 @@
       <c r="H217" s="34"/>
       <c r="I217" s="34"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="18"/>
       <c r="B218" s="34"/>
       <c r="C218" s="34"/>
@@ -4670,7 +4738,7 @@
       <c r="H218" s="34"/>
       <c r="I218" s="34"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="18"/>
       <c r="B219" s="34"/>
       <c r="C219" s="34"/>
@@ -4681,7 +4749,7 @@
       <c r="H219" s="34"/>
       <c r="I219" s="34"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="18"/>
       <c r="B220" s="34"/>
       <c r="C220" s="34"/>
@@ -4692,7 +4760,7 @@
       <c r="H220" s="34"/>
       <c r="I220" s="34"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="18"/>
       <c r="B221" s="34"/>
       <c r="C221" s="34"/>
@@ -4703,7 +4771,7 @@
       <c r="H221" s="34"/>
       <c r="I221" s="34"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="18"/>
       <c r="B222" s="34"/>
       <c r="C222" s="34"/>
@@ -4714,7 +4782,7 @@
       <c r="H222" s="34"/>
       <c r="I222" s="34"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="18"/>
       <c r="B223" s="34"/>
       <c r="C223" s="34"/>
@@ -4725,7 +4793,7 @@
       <c r="H223" s="34"/>
       <c r="I223" s="34"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="18"/>
       <c r="B224" s="34"/>
       <c r="C224" s="34"/>
@@ -4736,7 +4804,7 @@
       <c r="H224" s="34"/>
       <c r="I224" s="34"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="18"/>
       <c r="B225" s="34"/>
       <c r="C225" s="34"/>
@@ -4747,7 +4815,7 @@
       <c r="H225" s="34"/>
       <c r="I225" s="34"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="18"/>
       <c r="B226" s="34"/>
       <c r="C226" s="34"/>
@@ -4758,7 +4826,7 @@
       <c r="H226" s="34"/>
       <c r="I226" s="34"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="18"/>
       <c r="B227" s="34"/>
       <c r="C227" s="34"/>
@@ -4769,7 +4837,7 @@
       <c r="H227" s="34"/>
       <c r="I227" s="34"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="18"/>
       <c r="B228" s="34"/>
       <c r="C228" s="34"/>
@@ -4780,7 +4848,7 @@
       <c r="H228" s="34"/>
       <c r="I228" s="34"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="18"/>
       <c r="B229" s="34"/>
       <c r="C229" s="34"/>
@@ -4791,7 +4859,7 @@
       <c r="H229" s="34"/>
       <c r="I229" s="34"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="18"/>
       <c r="B230" s="34"/>
       <c r="C230" s="34"/>
@@ -4802,7 +4870,7 @@
       <c r="H230" s="34"/>
       <c r="I230" s="34"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="18"/>
       <c r="B231" s="34"/>
       <c r="C231" s="34"/>
@@ -4813,7 +4881,7 @@
       <c r="H231" s="34"/>
       <c r="I231" s="34"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="18"/>
       <c r="B232" s="34"/>
       <c r="C232" s="34"/>
@@ -4824,7 +4892,7 @@
       <c r="H232" s="34"/>
       <c r="I232" s="34"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="18"/>
       <c r="B233" s="34"/>
       <c r="C233" s="34"/>
@@ -4835,7 +4903,7 @@
       <c r="H233" s="34"/>
       <c r="I233" s="34"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="18"/>
       <c r="B234" s="34"/>
       <c r="C234" s="34"/>
@@ -4846,7 +4914,7 @@
       <c r="H234" s="34"/>
       <c r="I234" s="34"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="18"/>
       <c r="B235" s="34"/>
       <c r="C235" s="34"/>
@@ -4857,7 +4925,7 @@
       <c r="H235" s="34"/>
       <c r="I235" s="34"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="18"/>
       <c r="B236" s="34"/>
       <c r="C236" s="34"/>
@@ -4868,7 +4936,7 @@
       <c r="H236" s="34"/>
       <c r="I236" s="34"/>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="18"/>
       <c r="B237" s="34"/>
       <c r="C237" s="34"/>
@@ -4879,7 +4947,7 @@
       <c r="H237" s="34"/>
       <c r="I237" s="34"/>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="18"/>
       <c r="B238" s="34"/>
       <c r="C238" s="34"/>
@@ -4890,7 +4958,7 @@
       <c r="H238" s="34"/>
       <c r="I238" s="34"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="18"/>
       <c r="B239" s="34"/>
       <c r="C239" s="34"/>
@@ -4901,7 +4969,7 @@
       <c r="H239" s="34"/>
       <c r="I239" s="34"/>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="18"/>
       <c r="B240" s="34"/>
       <c r="C240" s="34"/>
@@ -4912,7 +4980,7 @@
       <c r="H240" s="34"/>
       <c r="I240" s="34"/>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="18"/>
       <c r="B241" s="34"/>
       <c r="C241" s="34"/>
@@ -4923,7 +4991,7 @@
       <c r="H241" s="34"/>
       <c r="I241" s="34"/>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="18"/>
       <c r="B242" s="34"/>
       <c r="C242" s="34"/>
@@ -4934,7 +5002,7 @@
       <c r="H242" s="34"/>
       <c r="I242" s="34"/>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="18"/>
       <c r="B243" s="34"/>
       <c r="C243" s="34"/>
@@ -4945,7 +5013,7 @@
       <c r="H243" s="34"/>
       <c r="I243" s="34"/>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="18"/>
       <c r="B244" s="34"/>
       <c r="C244" s="34"/>
@@ -4956,7 +5024,7 @@
       <c r="H244" s="34"/>
       <c r="I244" s="34"/>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="18"/>
       <c r="B245" s="34"/>
       <c r="C245" s="34"/>
@@ -4967,7 +5035,7 @@
       <c r="H245" s="34"/>
       <c r="I245" s="34"/>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="18"/>
       <c r="B246" s="34"/>
       <c r="C246" s="34"/>
@@ -4978,7 +5046,7 @@
       <c r="H246" s="34"/>
       <c r="I246" s="34"/>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="18"/>
       <c r="B247" s="34"/>
       <c r="C247" s="34"/>
@@ -4989,7 +5057,7 @@
       <c r="H247" s="34"/>
       <c r="I247" s="34"/>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="18"/>
       <c r="B248" s="34"/>
       <c r="C248" s="34"/>
@@ -5000,7 +5068,7 @@
       <c r="H248" s="34"/>
       <c r="I248" s="34"/>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="18"/>
       <c r="B249" s="34"/>
       <c r="C249" s="34"/>
@@ -5011,7 +5079,7 @@
       <c r="H249" s="34"/>
       <c r="I249" s="34"/>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="18"/>
       <c r="B250" s="34"/>
       <c r="C250" s="34"/>
@@ -5022,7 +5090,7 @@
       <c r="H250" s="34"/>
       <c r="I250" s="34"/>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="18"/>
       <c r="B251" s="34"/>
       <c r="C251" s="34"/>
@@ -5033,7 +5101,7 @@
       <c r="H251" s="34"/>
       <c r="I251" s="34"/>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="18"/>
       <c r="B252" s="34"/>
       <c r="C252" s="34"/>
@@ -5044,7 +5112,7 @@
       <c r="H252" s="34"/>
       <c r="I252" s="34"/>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="18"/>
       <c r="B253" s="34"/>
       <c r="C253" s="34"/>
@@ -5055,7 +5123,7 @@
       <c r="H253" s="34"/>
       <c r="I253" s="34"/>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="18"/>
       <c r="B254" s="34"/>
       <c r="C254" s="34"/>
@@ -5066,7 +5134,7 @@
       <c r="H254" s="34"/>
       <c r="I254" s="34"/>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="18"/>
       <c r="B255" s="34"/>
       <c r="C255" s="34"/>
@@ -5077,7 +5145,7 @@
       <c r="H255" s="34"/>
       <c r="I255" s="34"/>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="18"/>
       <c r="B256" s="34"/>
       <c r="C256" s="34"/>
@@ -5088,7 +5156,7 @@
       <c r="H256" s="34"/>
       <c r="I256" s="34"/>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="18"/>
       <c r="B257" s="34"/>
       <c r="C257" s="34"/>
@@ -5099,7 +5167,7 @@
       <c r="H257" s="34"/>
       <c r="I257" s="34"/>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="18"/>
       <c r="B258" s="34"/>
       <c r="C258" s="34"/>
@@ -5110,7 +5178,7 @@
       <c r="H258" s="34"/>
       <c r="I258" s="34"/>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="18"/>
       <c r="B259" s="34"/>
       <c r="C259" s="34"/>
@@ -5121,7 +5189,7 @@
       <c r="H259" s="34"/>
       <c r="I259" s="34"/>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="18"/>
       <c r="B260" s="34"/>
       <c r="C260" s="34"/>
@@ -5132,7 +5200,7 @@
       <c r="H260" s="34"/>
       <c r="I260" s="34"/>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="18"/>
       <c r="B261" s="34"/>
       <c r="C261" s="34"/>
@@ -5143,7 +5211,7 @@
       <c r="H261" s="34"/>
       <c r="I261" s="34"/>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="18"/>
       <c r="B262" s="34"/>
       <c r="C262" s="34"/>
@@ -5154,7 +5222,7 @@
       <c r="H262" s="34"/>
       <c r="I262" s="34"/>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="18"/>
       <c r="B263" s="34"/>
       <c r="C263" s="34"/>
@@ -5165,7 +5233,7 @@
       <c r="H263" s="34"/>
       <c r="I263" s="34"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="18"/>
       <c r="B264" s="34"/>
       <c r="C264" s="34"/>
@@ -5176,7 +5244,7 @@
       <c r="H264" s="34"/>
       <c r="I264" s="34"/>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="18"/>
       <c r="B265" s="34"/>
       <c r="C265" s="34"/>
@@ -5187,7 +5255,7 @@
       <c r="H265" s="34"/>
       <c r="I265" s="34"/>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="18"/>
       <c r="B266" s="34"/>
       <c r="C266" s="34"/>
@@ -5198,7 +5266,7 @@
       <c r="H266" s="34"/>
       <c r="I266" s="34"/>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="18"/>
       <c r="B267" s="34"/>
       <c r="C267" s="34"/>
@@ -5209,7 +5277,7 @@
       <c r="H267" s="34"/>
       <c r="I267" s="34"/>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="18"/>
       <c r="B268" s="34"/>
       <c r="C268" s="34"/>
@@ -5220,7 +5288,7 @@
       <c r="H268" s="34"/>
       <c r="I268" s="34"/>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="18"/>
       <c r="B269" s="34"/>
       <c r="C269" s="34"/>
@@ -5231,7 +5299,7 @@
       <c r="H269" s="34"/>
       <c r="I269" s="34"/>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="18"/>
       <c r="B270" s="34"/>
       <c r="C270" s="34"/>
@@ -5242,7 +5310,7 @@
       <c r="H270" s="34"/>
       <c r="I270" s="34"/>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="18"/>
       <c r="B271" s="34"/>
       <c r="C271" s="34"/>
@@ -5253,7 +5321,7 @@
       <c r="H271" s="34"/>
       <c r="I271" s="34"/>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="18"/>
       <c r="B272" s="34"/>
       <c r="C272" s="34"/>
@@ -5264,7 +5332,7 @@
       <c r="H272" s="34"/>
       <c r="I272" s="34"/>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="18"/>
       <c r="B273" s="34"/>
       <c r="C273" s="34"/>
@@ -5275,7 +5343,7 @@
       <c r="H273" s="34"/>
       <c r="I273" s="34"/>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="18"/>
       <c r="B274" s="34"/>
       <c r="C274" s="34"/>
@@ -5286,7 +5354,7 @@
       <c r="H274" s="34"/>
       <c r="I274" s="34"/>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="18"/>
       <c r="B275" s="34"/>
       <c r="C275" s="34"/>
@@ -5297,7 +5365,7 @@
       <c r="H275" s="34"/>
       <c r="I275" s="34"/>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="18"/>
       <c r="B276" s="34"/>
       <c r="C276" s="34"/>
@@ -5308,7 +5376,7 @@
       <c r="H276" s="34"/>
       <c r="I276" s="34"/>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="18"/>
       <c r="B277" s="34"/>
       <c r="C277" s="34"/>
@@ -5319,7 +5387,7 @@
       <c r="H277" s="34"/>
       <c r="I277" s="34"/>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="18"/>
       <c r="B278" s="34"/>
       <c r="C278" s="34"/>
@@ -5330,7 +5398,7 @@
       <c r="H278" s="34"/>
       <c r="I278" s="34"/>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="18"/>
       <c r="B279" s="34"/>
       <c r="C279" s="34"/>
@@ -5341,7 +5409,7 @@
       <c r="H279" s="34"/>
       <c r="I279" s="34"/>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="18"/>
       <c r="B280" s="34"/>
       <c r="C280" s="34"/>
@@ -5352,7 +5420,7 @@
       <c r="H280" s="34"/>
       <c r="I280" s="34"/>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="18"/>
       <c r="B281" s="17"/>
       <c r="C281" s="17"/>
@@ -5363,7 +5431,7 @@
       <c r="H281" s="20"/>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="18"/>
       <c r="B282" s="17"/>
       <c r="C282" s="17"/>
@@ -5372,7 +5440,7 @@
       <c r="F282" s="21"/>
       <c r="G282" s="21"/>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="18"/>
       <c r="B283" s="17"/>
       <c r="C283" s="17"/>
@@ -5381,7 +5449,7 @@
       <c r="F283" s="21"/>
       <c r="G283" s="21"/>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="18"/>
       <c r="B284" s="17"/>
       <c r="C284" s="17"/>
@@ -5390,7 +5458,7 @@
       <c r="F284" s="21"/>
       <c r="G284" s="21"/>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="18"/>
       <c r="B285" s="17"/>
       <c r="C285" s="17"/>
@@ -5399,7 +5467,7 @@
       <c r="F285" s="21"/>
       <c r="G285" s="21"/>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="18"/>
       <c r="B286" s="17"/>
       <c r="C286" s="17"/>
@@ -5408,7 +5476,7 @@
       <c r="F286" s="21"/>
       <c r="G286" s="21"/>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" s="18"/>
       <c r="B287" s="17"/>
       <c r="C287" s="17"/>
@@ -5417,7 +5485,7 @@
       <c r="F287" s="21"/>
       <c r="G287" s="21"/>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" s="18"/>
       <c r="B288" s="17"/>
       <c r="C288" s="17"/>
@@ -5426,7 +5494,7 @@
       <c r="F288" s="21"/>
       <c r="G288" s="21"/>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="18"/>
       <c r="B289" s="17"/>
       <c r="C289" s="17"/>
@@ -5435,7 +5503,7 @@
       <c r="F289" s="21"/>
       <c r="G289" s="21"/>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="18"/>
       <c r="B290" s="17"/>
       <c r="C290" s="17"/>
@@ -5444,7 +5512,7 @@
       <c r="F290" s="21"/>
       <c r="G290" s="21"/>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="18"/>
       <c r="B291" s="17"/>
       <c r="C291" s="17"/>
@@ -5453,7 +5521,7 @@
       <c r="F291" s="21"/>
       <c r="G291" s="21"/>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="18"/>
       <c r="B292" s="17"/>
       <c r="C292" s="17"/>
@@ -5462,7 +5530,7 @@
       <c r="F292" s="21"/>
       <c r="G292" s="21"/>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="18"/>
       <c r="B293" s="17"/>
       <c r="C293" s="17"/>
@@ -5471,7 +5539,7 @@
       <c r="F293" s="21"/>
       <c r="G293" s="21"/>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="18"/>
       <c r="B294" s="17"/>
       <c r="C294" s="17"/>
@@ -5480,7 +5548,7 @@
       <c r="F294" s="21"/>
       <c r="G294" s="21"/>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="18"/>
       <c r="B295" s="17"/>
       <c r="C295" s="17"/>
@@ -5489,7 +5557,7 @@
       <c r="F295" s="21"/>
       <c r="G295" s="21"/>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="18"/>
       <c r="B296" s="17"/>
       <c r="C296" s="17"/>
@@ -5498,7 +5566,7 @@
       <c r="F296" s="21"/>
       <c r="G296" s="21"/>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="18"/>
       <c r="B297" s="17"/>
       <c r="C297" s="17"/>
@@ -5507,7 +5575,7 @@
       <c r="F297" s="21"/>
       <c r="G297" s="21"/>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="18"/>
       <c r="B298" s="17"/>
       <c r="C298" s="17"/>
@@ -5516,7 +5584,7 @@
       <c r="F298" s="21"/>
       <c r="G298" s="21"/>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="18"/>
       <c r="B299" s="17"/>
       <c r="C299" s="17"/>
@@ -5525,7 +5593,7 @@
       <c r="F299" s="21"/>
       <c r="G299" s="21"/>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="18"/>
       <c r="B300" s="17"/>
       <c r="C300" s="17"/>
@@ -5534,7 +5602,7 @@
       <c r="F300" s="21"/>
       <c r="G300" s="21"/>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="18"/>
       <c r="B301" s="17"/>
       <c r="C301" s="17"/>
@@ -5543,7 +5611,7 @@
       <c r="F301" s="21"/>
       <c r="G301" s="21"/>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="18"/>
       <c r="B302" s="17"/>
       <c r="C302" s="17"/>
@@ -5552,7 +5620,7 @@
       <c r="F302" s="21"/>
       <c r="G302" s="21"/>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="18"/>
       <c r="B303" s="17"/>
       <c r="C303" s="17"/>
@@ -5561,7 +5629,7 @@
       <c r="F303" s="21"/>
       <c r="G303" s="21"/>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="18"/>
       <c r="B304" s="17"/>
       <c r="C304" s="17"/>
@@ -5570,7 +5638,7 @@
       <c r="F304" s="21"/>
       <c r="G304" s="21"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="19"/>
       <c r="B305" s="20"/>
       <c r="C305" s="20"/>
@@ -5605,37 +5673,37 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B4" sqref="B4:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="17.625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="45" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="46"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="47"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>12</v>
       </c>
@@ -5649,7 +5717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>75</v>
       </c>
@@ -5663,7 +5731,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>76</v>
       </c>
@@ -5677,7 +5745,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>77</v>
       </c>
@@ -5691,7 +5759,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>78</v>
       </c>
@@ -5705,10 +5773,10 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:D4"/>
@@ -5724,21 +5792,141 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255FB268-4FE2-48C7-9216-8EF72B402CAE}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="9">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:D11" xr:uid="{2FD4A490-92F2-4FE4-94B1-88A7806D90B4}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{79761EBD-6D3E-47F3-9C71-E1CA6187E2DF}">
+      <formula1>36526</formula1>
+      <formula2>401769</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -5752,7 +5940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
@@ -5763,7 +5951,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
@@ -5775,7 +5963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -5789,7 +5977,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -5800,7 +5988,7 @@
         <v>43877</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -5814,7 +6002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
@@ -5828,7 +6016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>84</v>
       </c>
@@ -5842,7 +6030,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
@@ -5853,7 +6041,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>38</v>
       </c>
@@ -5865,7 +6053,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>39</v>
       </c>
@@ -5876,7 +6064,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>40</v>
       </c>
@@ -5887,7 +6075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>41</v>
       </c>
@@ -5898,7 +6086,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>82</v>
       </c>

</xml_diff>